<commit_message>
Updated nearest tRNA-ribosome code
</commit_message>
<xml_diff>
--- a/calculations/tRNAChargingCalculations.xlsx
+++ b/calculations/tRNAChargingCalculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akshay/Documents/TranslationDynamics/calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15AF846B-BF72-6841-BC87-B78D2C4ADF4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6941EFD4-B872-D744-80D9-B409A8B7434C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="740" windowWidth="26440" windowHeight="15440" xr2:uid="{0CF1CF4C-15FC-784F-A1A5-5EA867F20012}"/>
+    <workbookView xWindow="80" yWindow="1060" windowWidth="29720" windowHeight="21180" xr2:uid="{0CF1CF4C-15FC-784F-A1A5-5EA867F20012}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>0.77dbl/hr</t>
   </si>
@@ -52,13 +52,52 @@
   </si>
   <si>
     <t>Ef-Tu</t>
+  </si>
+  <si>
+    <t>Neidhardt 1976</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-uniform tRNA charging: Avcilar-Kucukgoze et al. 2016 </t>
+  </si>
+  <si>
+    <t>Genomes</t>
+  </si>
+  <si>
+    <t>Schmidt 2016</t>
+  </si>
+  <si>
+    <t>Elongation factor Tu</t>
+  </si>
+  <si>
+    <t>Glucose</t>
+  </si>
+  <si>
+    <t>LB</t>
+  </si>
+  <si>
+    <t>Acetate</t>
+  </si>
+  <si>
+    <t>0.39dbl/hr</t>
+  </si>
+  <si>
+    <t>0.87 dbl/hr</t>
+  </si>
+  <si>
+    <t>2.3 dbl/hr</t>
+  </si>
+  <si>
+    <t>tRNA synth abundances (10 types)</t>
+  </si>
+  <si>
+    <t>Total tRNA synthetases</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -66,13 +105,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -87,8 +139,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,31 +458,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA7997F3-D1FC-3744-9A13-73FB2EE52D9F}">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="19.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" customWidth="1"/>
+    <col min="5" max="5" width="34.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>100</v>
-      </c>
-      <c r="C1">
-        <v>100</v>
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="C2">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="F2" t="s">
         <v>1</v>
@@ -444,10 +500,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="C3">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="F3">
         <v>192</v>
@@ -464,10 +520,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="C4">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F4">
         <v>297</v>
@@ -484,10 +540,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="C5">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="F5">
         <v>308</v>
@@ -504,10 +560,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="C6">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="F6">
         <v>222</v>
@@ -524,10 +580,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C7">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="F7">
         <v>425</v>
@@ -544,10 +600,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="C8">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="F8">
         <v>237</v>
@@ -564,10 +620,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="C9">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="F9">
         <v>132</v>
@@ -584,10 +640,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="C10">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="F10">
         <v>232</v>
@@ -604,10 +660,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="C11">
-        <v>100</v>
+        <v>34</v>
       </c>
       <c r="F11">
         <v>184</v>
@@ -624,10 +680,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="C12">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="F12">
         <v>155</v>
@@ -647,7 +703,7 @@
         <v>15</v>
       </c>
       <c r="C13">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="E13" t="s">
         <v>4</v>
@@ -675,11 +731,14 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C14">
         <v>55</v>
       </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
       <c r="F14">
         <v>1.5</v>
       </c>
@@ -695,10 +754,13 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C15">
-        <v>40</v>
+        <v>55</v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
       </c>
       <c r="F15">
         <f>F13*F14</f>
@@ -723,26 +785,26 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="C16">
         <v>40</v>
       </c>
-      <c r="C16">
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>40</v>
+      </c>
+      <c r="C17">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18">
         <v>30</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>35</v>
-      </c>
-      <c r="C18">
-        <v>55</v>
       </c>
       <c r="E18" t="s">
         <v>5</v>
@@ -760,12 +822,12 @@
         <v>76800</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="C19">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F19">
         <f>F14*F18</f>
@@ -783,117 +845,174 @@
         <f t="shared" si="2"/>
         <v>230400</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19">
+        <f>I19/F19</f>
+        <v>6.678260869565217</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
+        <v>90</v>
+      </c>
+      <c r="C20">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21">
         <v>80</v>
       </c>
-      <c r="C20">
+      <c r="C21">
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22">
         <v>60</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23">
         <v>70</v>
       </c>
-      <c r="C22">
+      <c r="C23">
         <v>75</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24">
         <v>80</v>
       </c>
-      <c r="C23">
+      <c r="C24">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25">
         <v>85</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <v>55</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="1">
+        <v>149278</v>
+      </c>
+      <c r="G25" s="1">
+        <v>252452</v>
+      </c>
+      <c r="I25" s="1">
+        <v>443852</v>
+      </c>
+      <c r="J25">
+        <f>I25/F25</f>
+        <v>2.9733249373651844</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26">
         <v>90</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <v>45</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>100</v>
-      </c>
-      <c r="C26">
+      <c r="E26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26">
+        <v>27537</v>
+      </c>
+      <c r="G26">
+        <v>47373</v>
+      </c>
+      <c r="I26">
+        <v>76836</v>
+      </c>
+      <c r="J26">
+        <f>I26/F26</f>
+        <v>2.7902821658132693</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>100</v>
+      </c>
+      <c r="C27">
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>100</v>
-      </c>
-      <c r="C27">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>100</v>
+      </c>
+      <c r="C28">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29">
         <v>95</v>
       </c>
-      <c r="C28">
+      <c r="C29">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>100</v>
-      </c>
-      <c r="C29">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>100</v>
+      </c>
+      <c r="C30">
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>100</v>
-      </c>
-      <c r="C30">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>100</v>
+      </c>
+      <c r="C31">
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32">
         <v>90</v>
       </c>
-      <c r="C31">
+      <c r="C32">
         <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>55</v>
-      </c>
-      <c r="C32">
-        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C33">
-        <v>85</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -901,7 +1020,7 @@
         <v>60</v>
       </c>
       <c r="C34">
-        <v>70</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -909,7 +1028,7 @@
         <v>60</v>
       </c>
       <c r="C35">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -917,45 +1036,53 @@
         <v>60</v>
       </c>
       <c r="C36">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="C37">
-        <v>60</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C38">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C39">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>100</v>
+        <v>75</v>
+      </c>
+      <c r="C40">
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
-        <f>AVERAGE(A1:A40)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <f>AVERAGE(A2:A41)</f>
         <v>68.5</v>
       </c>
-      <c r="C41">
-        <f>AVERAGE(C1:C39)</f>
+      <c r="C42">
+        <f>AVERAGE(C2:C40)</f>
         <v>61.128205128205131</v>
       </c>
     </row>

</xml_diff>